<commit_message>
warning + pref tab update
Also made weight % for static ingredients fixed
</commit_message>
<xml_diff>
--- a/Restored To Eden/Formulation Templates/Oil Serum Worksheet.xlsx
+++ b/Restored To Eden/Formulation Templates/Oil Serum Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\source\repos\ingredient-sorter\Restored To Eden\Formulation Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E54703-7099-4904-A903-5B925E6461C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C901FAA7-48D2-4447-948B-302F22B3DDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="-15285" windowWidth="17130" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t xml:space="preserve">Customer Name  </t>
   </si>
@@ -114,13 +114,7 @@
     <t>EO Base</t>
   </si>
   <si>
-    <t xml:space="preserve">EO Top, Middle or Base </t>
-  </si>
-  <si>
     <t>Antioxidant [this ingredient doesn't change]</t>
-  </si>
-  <si>
-    <t>Anhydrous high performance</t>
   </si>
   <si>
     <t>TOTAL 100%</t>
@@ -280,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -305,9 +299,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -639,11 +630,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AB997"/>
+  <dimension ref="A1:AB993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -696,19 +687,19 @@
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -734,17 +725,17 @@
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -770,17 +761,17 @@
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -812,10 +803,10 @@
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
@@ -1135,7 +1126,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -1166,7 +1157,9 @@
       <c r="C15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10">
+        <v>0.5</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1193,16 +1186,15 @@
     </row>
     <row r="16" spans="1:28" ht="17.399999999999999">
       <c r="A16" s="12"/>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>23</v>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16">
+        <f>SUM(D7:D15)</f>
+        <v>100</v>
       </c>
-      <c r="D16" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="I16" s="4"/>
@@ -1226,16 +1218,11 @@
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
     </row>
-    <row r="17" spans="1:28" ht="17.399999999999999">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+    <row r="17" spans="1:28" ht="36.75" customHeight="1">
+      <c r="A17" s="18"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="I17" s="4"/>
@@ -1260,17 +1247,14 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28" ht="17.399999999999999">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1293,17 +1277,14 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28" ht="17.399999999999999">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
@@ -1326,18 +1307,14 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28" ht="17.399999999999999">
-      <c r="A20" s="12"/>
-      <c r="B20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17">
-        <f>SUM(D7:D19)</f>
-        <v>100</v>
-      </c>
-      <c r="E20" s="18"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1359,13 +1336,15 @@
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
     </row>
-    <row r="21" spans="1:28" ht="36.75" customHeight="1">
-      <c r="A21" s="19"/>
+    <row r="21" spans="1:28" ht="17.399999999999999">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -30547,126 +30526,6 @@
       <c r="AA993" s="4"/>
       <c r="AB993" s="4"/>
     </row>
-    <row r="994" spans="1:28" ht="17.399999999999999">
-      <c r="A994" s="4"/>
-      <c r="B994" s="4"/>
-      <c r="C994" s="4"/>
-      <c r="D994" s="4"/>
-      <c r="E994" s="4"/>
-      <c r="F994" s="4"/>
-      <c r="G994" s="4"/>
-      <c r="H994" s="4"/>
-      <c r="I994" s="4"/>
-      <c r="J994" s="4"/>
-      <c r="K994" s="4"/>
-      <c r="L994" s="4"/>
-      <c r="M994" s="4"/>
-      <c r="N994" s="4"/>
-      <c r="O994" s="4"/>
-      <c r="P994" s="4"/>
-      <c r="Q994" s="4"/>
-      <c r="R994" s="4"/>
-      <c r="S994" s="4"/>
-      <c r="T994" s="4"/>
-      <c r="U994" s="4"/>
-      <c r="V994" s="4"/>
-      <c r="W994" s="4"/>
-      <c r="X994" s="4"/>
-      <c r="Y994" s="4"/>
-      <c r="Z994" s="4"/>
-      <c r="AA994" s="4"/>
-      <c r="AB994" s="4"/>
-    </row>
-    <row r="995" spans="1:28" ht="17.399999999999999">
-      <c r="A995" s="4"/>
-      <c r="B995" s="4"/>
-      <c r="C995" s="4"/>
-      <c r="D995" s="4"/>
-      <c r="E995" s="4"/>
-      <c r="F995" s="4"/>
-      <c r="G995" s="4"/>
-      <c r="H995" s="4"/>
-      <c r="I995" s="4"/>
-      <c r="J995" s="4"/>
-      <c r="K995" s="4"/>
-      <c r="L995" s="4"/>
-      <c r="M995" s="4"/>
-      <c r="N995" s="4"/>
-      <c r="O995" s="4"/>
-      <c r="P995" s="4"/>
-      <c r="Q995" s="4"/>
-      <c r="R995" s="4"/>
-      <c r="S995" s="4"/>
-      <c r="T995" s="4"/>
-      <c r="U995" s="4"/>
-      <c r="V995" s="4"/>
-      <c r="W995" s="4"/>
-      <c r="X995" s="4"/>
-      <c r="Y995" s="4"/>
-      <c r="Z995" s="4"/>
-      <c r="AA995" s="4"/>
-      <c r="AB995" s="4"/>
-    </row>
-    <row r="996" spans="1:28" ht="17.399999999999999">
-      <c r="A996" s="4"/>
-      <c r="B996" s="4"/>
-      <c r="C996" s="4"/>
-      <c r="D996" s="4"/>
-      <c r="E996" s="4"/>
-      <c r="F996" s="4"/>
-      <c r="G996" s="4"/>
-      <c r="H996" s="4"/>
-      <c r="I996" s="4"/>
-      <c r="J996" s="4"/>
-      <c r="K996" s="4"/>
-      <c r="L996" s="4"/>
-      <c r="M996" s="4"/>
-      <c r="N996" s="4"/>
-      <c r="O996" s="4"/>
-      <c r="P996" s="4"/>
-      <c r="Q996" s="4"/>
-      <c r="R996" s="4"/>
-      <c r="S996" s="4"/>
-      <c r="T996" s="4"/>
-      <c r="U996" s="4"/>
-      <c r="V996" s="4"/>
-      <c r="W996" s="4"/>
-      <c r="X996" s="4"/>
-      <c r="Y996" s="4"/>
-      <c r="Z996" s="4"/>
-      <c r="AA996" s="4"/>
-      <c r="AB996" s="4"/>
-    </row>
-    <row r="997" spans="1:28" ht="17.399999999999999">
-      <c r="A997" s="4"/>
-      <c r="B997" s="4"/>
-      <c r="C997" s="4"/>
-      <c r="D997" s="4"/>
-      <c r="E997" s="4"/>
-      <c r="F997" s="4"/>
-      <c r="G997" s="4"/>
-      <c r="H997" s="4"/>
-      <c r="I997" s="4"/>
-      <c r="J997" s="4"/>
-      <c r="K997" s="4"/>
-      <c r="L997" s="4"/>
-      <c r="M997" s="4"/>
-      <c r="N997" s="4"/>
-      <c r="O997" s="4"/>
-      <c r="P997" s="4"/>
-      <c r="Q997" s="4"/>
-      <c r="R997" s="4"/>
-      <c r="S997" s="4"/>
-      <c r="T997" s="4"/>
-      <c r="U997" s="4"/>
-      <c r="V997" s="4"/>
-      <c r="W997" s="4"/>
-      <c r="X997" s="4"/>
-      <c r="Y997" s="4"/>
-      <c r="Z997" s="4"/>
-      <c r="AA997" s="4"/>
-      <c r="AB997" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C2:E2"/>

</xml_diff>